<commit_message>
added annotations on Findbugs heuristics
</commit_message>
<xml_diff>
--- a/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
+++ b/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
@@ -1,16 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="0" windowWidth="33000" windowHeight="23420" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4215" yWindow="0" windowWidth="20730" windowHeight="23415" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analyses" sheetId="1" r:id="rId1"/>
     <sheet name="ausgewählte Analysen" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="DL_SYNCHRONIZATION_ON_BOXED_PRIMITIVE" localSheetId="1">'ausgewählte Analysen'!$C$17</definedName>
+    <definedName name="DMI_LONG_BITS_TO_DOUBLE_INVOKED_ON_INT" localSheetId="1">'ausgewählte Analysen'!$C$15</definedName>
+    <definedName name="ITA_INEFFICIENT_TO_ARRAY" localSheetId="1">'ausgewählte Analysen'!$C$14</definedName>
+    <definedName name="MS_PKGPROTECT" localSheetId="1">'ausgewählte Analysen'!$C$16</definedName>
+    <definedName name="RC_REF_COMPARISON" localSheetId="1">'ausgewählte Analysen'!$C$11</definedName>
+    <definedName name="SA_LOCAL_SELF_ASSIGNMENT_INSTEAD_OF_FIELD" localSheetId="1">'ausgewählte Analysen'!$C$19</definedName>
+    <definedName name="SIC_INNER_SHOULD_BE_STATIC_ANON" localSheetId="1">'ausgewählte Analysen'!$C$12</definedName>
+    <definedName name="SQL_BAD_PREPARED_STATEMENT_ACCESS" localSheetId="1">'ausgewählte Analysen'!$C$13</definedName>
+    <definedName name="UR_UNINIT_READ_CALLED_FROM_SUPER_CONSTRUCTOR" localSheetId="1">'ausgewählte Analysen'!$C$18</definedName>
+  </definedNames>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="451">
   <si>
     <t>AM: Creates an empty jar file entry</t>
   </si>
@@ -1324,12 +1335,72 @@
   <si>
     <t>???????</t>
   </si>
+  <si>
+    <t>Found In</t>
+  </si>
+  <si>
+    <t>Hibernate 3.6.6.</t>
+  </si>
+  <si>
+    <t>Hibernate 3.6.6. (but as named class not as anonymous)</t>
+  </si>
+  <si>
+    <t>FindBug Heuristic</t>
+  </si>
+  <si>
+    <t>count aload_1  &gt; 1 (this could make sense, given that the compiler generates code to initialize the field for referencing outer.this, then the end-user's value is most probably retrieved via another aload_1)</t>
+  </si>
+  <si>
+    <t>RC_REF_COMPARISON</t>
+  </si>
+  <si>
+    <t>SIC_INNER_SHOULD_BE_STATIC_ANON</t>
+  </si>
+  <si>
+    <t>SQL_BAD_PREPARED_STATEMENT_ACCESS</t>
+  </si>
+  <si>
+    <t>INVOKEINTERFACE with set/get/update and a fixed list of suffixes</t>
+  </si>
+  <si>
+    <t>ITA_INEFFICIENT_TO_ARRAY</t>
+  </si>
+  <si>
+    <t>opcode sequence of ICONST_0, ANEWARRAY, INVOKE…</t>
+  </si>
+  <si>
+    <t>!!! NOT FOUND IN MY TESTCASE !!!</t>
+  </si>
+  <si>
+    <t>DMI_LONG_BITS_TO_DOUBLE_INVOKED_ON_INT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i2l before call </t>
+  </si>
+  <si>
+    <t>MS_PKGPROTECT</t>
+  </si>
+  <si>
+    <t>Reports a bug if: field is public/protected static final Array or Hashtable and not used from a different package (other use cases are reported as different bugs, e.g., usage outside of the packge)</t>
+  </si>
+  <si>
+    <t>DL_SYNCHRONIZATION_ON_BOXED_PRIMITIVE</t>
+  </si>
+  <si>
+    <t>UR_UNINIT_READ_CALLED_FROM_SUPER_CONSTRUCTOR</t>
+  </si>
+  <si>
+    <t>SA_LOCAL_SELF_ASSIGNMENT_INSTEAD_OF_FIELD</t>
+  </si>
+  <si>
+    <t>Selfwritten DF analysis; loops over instructions, saves branch targets and counts goto's</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1413,7 +1484,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1423,6 +1494,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1461,7 +1538,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1471,19 +1548,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1495,10 +1573,15 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1826,13 +1909,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C401"/>
   <sheetViews>
-    <sheetView topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="90.1640625" customWidth="1"/>
+    <col min="2" max="2" width="90.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6260,63 +6343,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:H226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="2" max="2" width="71.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.625" customWidth="1"/>
+    <col min="2" max="2" width="71.375" customWidth="1"/>
+    <col min="3" max="3" width="29.625" customWidth="1"/>
+    <col min="6" max="6" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>414</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>409</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1">
+    <row r="5" spans="1:8" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10" t="s">
+        <v>431</v>
+      </c>
+      <c r="H10" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>186</v>
       </c>
@@ -6325,10 +6417,13 @@
         <v>RC: Suspicious reference comparison</v>
       </c>
       <c r="C11" t="s">
+        <v>436</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>312</v>
       </c>
@@ -6337,10 +6432,19 @@
         <v>SIC: Could be refactored into a named static inner class</v>
       </c>
       <c r="C12" t="s">
+        <v>437</v>
+      </c>
+      <c r="D12" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="G12" t="s">
+        <v>433</v>
+      </c>
+      <c r="H12" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>208</v>
       </c>
@@ -6349,10 +6453,16 @@
         <v>SQL: Method attempts to access a prepared statement parameter with index 0</v>
       </c>
       <c r="C13" t="s">
+        <v>438</v>
+      </c>
+      <c r="D13" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="H13" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>309</v>
       </c>
@@ -6361,10 +6471,19 @@
         <v>ITA: Method uses toArray() with zero-length array argument</v>
       </c>
       <c r="C14" t="s">
+        <v>440</v>
+      </c>
+      <c r="D14" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="G14" t="s">
+        <v>442</v>
+      </c>
+      <c r="H14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>109</v>
       </c>
@@ -6373,10 +6492,16 @@
         <v>DMI: Double.longBitsToDouble invoked on an int</v>
       </c>
       <c r="C15" t="s">
+        <v>443</v>
+      </c>
+      <c r="D15" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="16">
+      <c r="H15" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>245</v>
       </c>
@@ -6384,11 +6509,14 @@
         <f>LOOKUP(A16,Analyses!$A$1:$B$401)</f>
         <v>MS: Field should be package protected</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="C16" t="s">
+        <v>445</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>251</v>
       </c>
@@ -6397,10 +6525,13 @@
         <v>DL: Synchronization on boxed primitive</v>
       </c>
       <c r="C17" t="s">
+        <v>447</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>221</v>
       </c>
@@ -6408,11 +6539,14 @@
         <f>LOOKUP(A18,Analyses!$A$1:$B$401)</f>
         <v>UR: Uninitialized read of field method called from constructor of superclass</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
+        <v>448</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>201</v>
       </c>
@@ -6421,10 +6555,16 @@
         <v>SA: Self assignment of local rather than assignment to field</v>
       </c>
       <c r="C19" t="s">
+        <v>449</v>
+      </c>
+      <c r="D19" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="H19" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>73</v>
       </c>
@@ -6432,11 +6572,11 @@
         <f>LOOKUP(A20,Analyses!$A$1:$B$401)</f>
         <v>Se: Non-serializable class has a serializable inner class</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>177</v>
       </c>
@@ -6444,11 +6584,11 @@
         <f>LOOKUP(A21,Analyses!$A$1:$B$401)</f>
         <v>NP: Store of null value into field annotated NonNull</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>30</v>
       </c>
@@ -6456,11 +6596,11 @@
         <f>LOOKUP(A22,Analyses!$A$1:$B$401)</f>
         <v>FI: Finalizer does nothing but call superclass finalizer</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>71</v>
       </c>
@@ -6468,11 +6608,11 @@
         <f>LOOKUP(A23,Analyses!$A$1:$B$401)</f>
         <v>SW: Certain swing methods needs to be invoked in Swing thread</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>267</v>
       </c>
@@ -6480,11 +6620,11 @@
         <f>LOOKUP(A24,Analyses!$A$1:$B$401)</f>
         <v>MWN: Mismatched notify()</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>246</v>
       </c>
@@ -6492,11 +6632,11 @@
         <f>LOOKUP(A25,Analyses!$A$1:$B$401)</f>
         <v>MS: Field isn't final but should be</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>234</v>
       </c>
@@ -6504,11 +6644,11 @@
         <f>LOOKUP(A26,Analyses!$A$1:$B$401)</f>
         <v>DP: Method invoked that should be only be invoked inside a doPrivileged block</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>387</v>
       </c>
@@ -6516,11 +6656,11 @@
         <f>LOOKUP(A27,Analyses!$A$1:$B$401)</f>
         <v>SA: Self assignment of local variable</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>199</v>
       </c>
@@ -6528,11 +6668,11 @@
         <f>LOOKUP(A28,Analyses!$A$1:$B$401)</f>
         <v>SA: Self comparison of field with itself</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>294</v>
       </c>
@@ -6540,11 +6680,11 @@
         <f>LOOKUP(A29,Analyses!$A$1:$B$401)</f>
         <v>Bx: Primitive value is boxed then unboxed to perform primitive coercion</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>223</v>
       </c>
@@ -6552,11 +6692,14 @@
         <f>LOOKUP(A30,Analyses!$A$1:$B$401)</f>
         <v>USELESS_STRING: Invocation of toString on an array</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="G30" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>196</v>
       </c>
@@ -6564,11 +6707,11 @@
         <f>LOOKUP(A31,Analyses!$A$1:$B$401)</f>
         <v>RV: Method ignores return value</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>69</v>
       </c>
@@ -6576,11 +6719,11 @@
         <f>LOOKUP(A32,Analyses!$A$1:$B$401)</f>
         <v>RV: Method ignores exceptional return value</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>283</v>
       </c>
@@ -6588,11 +6731,11 @@
         <f>LOOKUP(A33,Analyses!$A$1:$B$401)</f>
         <v>UG: Unsynchronized get method, synchronized set method</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>10</v>
       </c>
@@ -6600,11 +6743,11 @@
         <f>LOOKUP(A34,Analyses!$A$1:$B$401)</f>
         <v>DE: Method might drop exception</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="7" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>151</v>
       </c>
@@ -6612,11 +6755,11 @@
         <f>LOOKUP(A35,Analyses!$A$1:$B$401)</f>
         <v>IL: A collection is added to itself</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>320</v>
       </c>
@@ -6624,11 +6767,11 @@
         <f>LOOKUP(A36,Analyses!$A$1:$B$401)</f>
         <v>Dm: Hardcoded constant database password</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>342</v>
       </c>
@@ -6636,11 +6779,11 @@
         <f>LOOKUP(A37,Analyses!$A$1:$B$401)</f>
         <v>DLS: Dead store of null to local variable</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>41</v>
       </c>
@@ -6648,11 +6791,11 @@
         <f>LOOKUP(A38,Analyses!$A$1:$B$401)</f>
         <v>It: Iterator next() method can't throw NoSuchElementException</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="7" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>393</v>
       </c>
@@ -6660,11 +6803,11 @@
         <f>LOOKUP(A39,Analyses!$A$1:$B$401)</f>
         <v>TQ: Value required to have type qualifier, but marked as unknown</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>105</v>
       </c>
@@ -6672,11 +6815,11 @@
         <f>LOOKUP(A40,Analyses!$A$1:$B$401)</f>
         <v>DMI: hasNext method invokes next</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>305</v>
       </c>
@@ -6684,11 +6827,11 @@
         <f>LOOKUP(A41,Analyses!$A$1:$B$401)</f>
         <v>Dm: Method invokes inefficient new String(String) constructor</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>110</v>
       </c>
@@ -6697,7 +6840,7 @@
         <v>DMI: Vacuous call to collections</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>62</v>
       </c>
@@ -6706,7 +6849,7 @@
         <v>OS: Method may fail to close stream on exception</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>328</v>
       </c>
@@ -6715,7 +6858,7 @@
         <v>XSS: JSP reflected cross site scripting vulnerability</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>147</v>
       </c>
@@ -6724,7 +6867,7 @@
         <v>IJU: TestCase has no tests</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>17</v>
       </c>
@@ -6733,7 +6876,7 @@
         <v>ES: Comparison of String parameter using == or !=</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>248</v>
       </c>
@@ -6742,7 +6885,7 @@
         <v>AT: Sequence of calls to concurrent abstraction may not be atomic</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>189</v>
       </c>
@@ -7819,7 +7962,7 @@
     <sortCondition ref="A127"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added a column to mark the current state of the implementation of a checker
</commit_message>
<xml_diff>
--- a/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
+++ b/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="0" windowWidth="20730" windowHeight="23415" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-38300" yWindow="-380" windowWidth="38320" windowHeight="23560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analyses" sheetId="1" r:id="rId1"/>
     <sheet name="ausgewählte Analysen" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DL_SYNCHRONIZATION_ON_BOXED_PRIMITIVE" localSheetId="1">'ausgewählte Analysen'!$C$17</definedName>
-    <definedName name="DMI_LONG_BITS_TO_DOUBLE_INVOKED_ON_INT" localSheetId="1">'ausgewählte Analysen'!$C$15</definedName>
-    <definedName name="ITA_INEFFICIENT_TO_ARRAY" localSheetId="1">'ausgewählte Analysen'!$C$14</definedName>
-    <definedName name="MS_PKGPROTECT" localSheetId="1">'ausgewählte Analysen'!$C$16</definedName>
-    <definedName name="RC_REF_COMPARISON" localSheetId="1">'ausgewählte Analysen'!$C$11</definedName>
-    <definedName name="SA_LOCAL_SELF_ASSIGNMENT_INSTEAD_OF_FIELD" localSheetId="1">'ausgewählte Analysen'!$C$19</definedName>
-    <definedName name="SIC_INNER_SHOULD_BE_STATIC_ANON" localSheetId="1">'ausgewählte Analysen'!$C$12</definedName>
-    <definedName name="SQL_BAD_PREPARED_STATEMENT_ACCESS" localSheetId="1">'ausgewählte Analysen'!$C$13</definedName>
-    <definedName name="UR_UNINIT_READ_CALLED_FROM_SUPER_CONSTRUCTOR" localSheetId="1">'ausgewählte Analysen'!$C$18</definedName>
+    <definedName name="DL_SYNCHRONIZATION_ON_BOXED_PRIMITIVE" localSheetId="1">'ausgewählte Analysen'!$D$17</definedName>
+    <definedName name="DMI_LONG_BITS_TO_DOUBLE_INVOKED_ON_INT" localSheetId="1">'ausgewählte Analysen'!$D$15</definedName>
+    <definedName name="ITA_INEFFICIENT_TO_ARRAY" localSheetId="1">'ausgewählte Analysen'!$D$14</definedName>
+    <definedName name="MS_PKGPROTECT" localSheetId="1">'ausgewählte Analysen'!$D$16</definedName>
+    <definedName name="RC_REF_COMPARISON" localSheetId="1">'ausgewählte Analysen'!$D$11</definedName>
+    <definedName name="SA_LOCAL_SELF_ASSIGNMENT_INSTEAD_OF_FIELD" localSheetId="1">'ausgewählte Analysen'!$D$19</definedName>
+    <definedName name="SIC_INNER_SHOULD_BE_STATIC_ANON" localSheetId="1">'ausgewählte Analysen'!$D$12</definedName>
+    <definedName name="SQL_BAD_PREPARED_STATEMENT_ACCESS" localSheetId="1">'ausgewählte Analysen'!$D$13</definedName>
+    <definedName name="UR_UNINIT_READ_CALLED_FROM_SUPER_CONSTRUCTOR" localSheetId="1">'ausgewählte Analysen'!$D$18</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="454">
   <si>
     <t>AM: Creates an empty jar file entry</t>
   </si>
@@ -1395,12 +1395,21 @@
   <si>
     <t>Selfwritten DF analysis; loops over instructions, saves branch targets and counts goto's</t>
   </si>
+  <si>
+    <t>SE_BAD_FIELD_INNER_CLASS</t>
+  </si>
+  <si>
+    <t>NP_STORE_INTO_NONNULL_FIELD</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1483,6 +1492,25 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Zapf Dingbats"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1538,7 +1566,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1549,19 +1577,22 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1573,7 +1604,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1913,9 +1944,9 @@
       <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="90.125" customWidth="1"/>
+    <col min="2" max="2" width="90.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6343,1111 +6374,1125 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H226"/>
+  <dimension ref="A1:I226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="31.625" customWidth="1"/>
-    <col min="2" max="2" width="71.375" customWidth="1"/>
-    <col min="3" max="3" width="29.625" customWidth="1"/>
-    <col min="6" max="6" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="71.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" ht="16">
       <c r="A1" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="1"/>
+      <c r="E1" t="s">
         <v>414</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>409</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1">
+    <row r="5" spans="1:9" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9" ht="16">
       <c r="A10" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="G10" t="s">
+      <c r="B10" s="1"/>
+      <c r="H10" t="s">
         <v>431</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>186</v>
       </c>
-      <c r="B11" t="str">
+      <c r="C11" t="str">
         <f>LOOKUP(A11,Analyses!$A$1:$B$401)</f>
         <v>RC: Suspicious reference comparison</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>436</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>312</v>
       </c>
-      <c r="B12" t="str">
+      <c r="C12" t="str">
         <f>LOOKUP(A12,Analyses!$A$1:$B$401)</f>
         <v>SIC: Could be refactored into a named static inner class</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>437</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>416</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>433</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>208</v>
       </c>
-      <c r="B13" t="str">
+      <c r="C13" t="str">
         <f>LOOKUP(A13,Analyses!$A$1:$B$401)</f>
         <v>SQL: Method attempts to access a prepared statement parameter with index 0</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>438</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>417</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>309</v>
       </c>
-      <c r="B14" t="str">
+      <c r="C14" t="str">
         <f>LOOKUP(A14,Analyses!$A$1:$B$401)</f>
         <v>ITA: Method uses toArray() with zero-length array argument</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>440</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>418</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>442</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>109</v>
       </c>
-      <c r="B15" t="str">
+      <c r="C15" t="str">
         <f>LOOKUP(A15,Analyses!$A$1:$B$401)</f>
         <v>DMI: Double.longBitsToDouble invoked on an int</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>443</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>419</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9" ht="16">
       <c r="A16">
         <v>245</v>
       </c>
-      <c r="B16" t="str">
+      <c r="C16" t="str">
         <f>LOOKUP(A16,Analyses!$A$1:$B$401)</f>
         <v>MS: Field should be package protected</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>445</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>251</v>
       </c>
-      <c r="B17" t="str">
+      <c r="C17" t="str">
         <f>LOOKUP(A17,Analyses!$A$1:$B$401)</f>
         <v>DL: Synchronization on boxed primitive</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>447</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>221</v>
       </c>
-      <c r="B18" t="str">
+      <c r="C18" t="str">
         <f>LOOKUP(A18,Analyses!$A$1:$B$401)</f>
         <v>UR: Uninitialized read of field method called from constructor of superclass</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>448</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>201</v>
       </c>
-      <c r="B19" t="str">
+      <c r="C19" t="str">
         <f>LOOKUP(A19,Analyses!$A$1:$B$401)</f>
         <v>SA: Self assignment of local rather than assignment to field</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>449</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>421</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20">
+    <row r="20" spans="1:9" s="10" customFormat="1">
+      <c r="A20" s="10">
         <v>73</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B20" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="C20" s="10" t="str">
         <f>LOOKUP(A20,Analyses!$A$1:$B$401)</f>
         <v>Se: Non-serializable class has a serializable inner class</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21">
+    <row r="21" spans="1:9" s="12" customFormat="1">
+      <c r="A21" s="12">
         <v>177</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B21" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C21" s="12" t="str">
         <f>LOOKUP(A21,Analyses!$A$1:$B$401)</f>
         <v>NP: Store of null value into field annotated NonNull</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>30</v>
       </c>
-      <c r="B22" t="str">
+      <c r="C22" t="str">
         <f>LOOKUP(A22,Analyses!$A$1:$B$401)</f>
         <v>FI: Finalizer does nothing but call superclass finalizer</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9" ht="16">
       <c r="A23">
         <v>71</v>
       </c>
-      <c r="B23" t="str">
+      <c r="C23" t="str">
         <f>LOOKUP(A23,Analyses!$A$1:$B$401)</f>
         <v>SW: Certain swing methods needs to be invoked in Swing thread</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>267</v>
       </c>
-      <c r="B24" t="str">
+      <c r="C24" t="str">
         <f>LOOKUP(A24,Analyses!$A$1:$B$401)</f>
         <v>MWN: Mismatched notify()</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9" ht="16">
       <c r="A25">
         <v>246</v>
       </c>
-      <c r="B25" t="str">
+      <c r="C25" t="str">
         <f>LOOKUP(A25,Analyses!$A$1:$B$401)</f>
         <v>MS: Field isn't final but should be</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9" ht="16">
       <c r="A26">
         <v>234</v>
       </c>
-      <c r="B26" t="str">
+      <c r="C26" t="str">
         <f>LOOKUP(A26,Analyses!$A$1:$B$401)</f>
         <v>DP: Method invoked that should be only be invoked inside a doPrivileged block</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9" ht="16">
       <c r="A27">
         <v>387</v>
       </c>
-      <c r="B27" t="str">
+      <c r="C27" t="str">
         <f>LOOKUP(A27,Analyses!$A$1:$B$401)</f>
         <v>SA: Self assignment of local variable</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>199</v>
       </c>
-      <c r="B28" t="str">
+      <c r="C28" t="str">
         <f>LOOKUP(A28,Analyses!$A$1:$B$401)</f>
         <v>SA: Self comparison of field with itself</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>294</v>
       </c>
-      <c r="B29" t="str">
+      <c r="C29" t="str">
         <f>LOOKUP(A29,Analyses!$A$1:$B$401)</f>
         <v>Bx: Primitive value is boxed then unboxed to perform primitive coercion</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>223</v>
       </c>
-      <c r="B30" t="str">
+      <c r="C30" t="str">
         <f>LOOKUP(A30,Analyses!$A$1:$B$401)</f>
         <v>USELESS_STRING: Invocation of toString on an array</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>196</v>
       </c>
-      <c r="B31" t="str">
+      <c r="C31" t="str">
         <f>LOOKUP(A31,Analyses!$A$1:$B$401)</f>
         <v>RV: Method ignores return value</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9" ht="16">
       <c r="A32">
         <v>69</v>
       </c>
-      <c r="B32" t="str">
+      <c r="C32" t="str">
         <f>LOOKUP(A32,Analyses!$A$1:$B$401)</f>
         <v>RV: Method ignores exceptional return value</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>283</v>
       </c>
-      <c r="B33" t="str">
+      <c r="C33" t="str">
         <f>LOOKUP(A33,Analyses!$A$1:$B$401)</f>
         <v>UG: Unsynchronized get method, synchronized set method</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5" ht="16">
       <c r="A34">
         <v>10</v>
       </c>
-      <c r="B34" t="str">
+      <c r="C34" t="str">
         <f>LOOKUP(A34,Analyses!$A$1:$B$401)</f>
         <v>DE: Method might drop exception</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>151</v>
       </c>
-      <c r="B35" t="str">
+      <c r="C35" t="str">
         <f>LOOKUP(A35,Analyses!$A$1:$B$401)</f>
         <v>IL: A collection is added to itself</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>320</v>
       </c>
-      <c r="B36" t="str">
+      <c r="C36" t="str">
         <f>LOOKUP(A36,Analyses!$A$1:$B$401)</f>
         <v>Dm: Hardcoded constant database password</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>342</v>
       </c>
-      <c r="B37" t="str">
+      <c r="C37" t="str">
         <f>LOOKUP(A37,Analyses!$A$1:$B$401)</f>
         <v>DLS: Dead store of null to local variable</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5" ht="16">
       <c r="A38">
         <v>41</v>
       </c>
-      <c r="B38" t="str">
+      <c r="C38" t="str">
         <f>LOOKUP(A38,Analyses!$A$1:$B$401)</f>
         <v>It: Iterator next() method can't throw NoSuchElementException</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="E38" s="7" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>393</v>
       </c>
-      <c r="B39" t="str">
+      <c r="C39" t="str">
         <f>LOOKUP(A39,Analyses!$A$1:$B$401)</f>
         <v>TQ: Value required to have type qualifier, but marked as unknown</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>105</v>
       </c>
-      <c r="B40" t="str">
+      <c r="C40" t="str">
         <f>LOOKUP(A40,Analyses!$A$1:$B$401)</f>
         <v>DMI: hasNext method invokes next</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>305</v>
       </c>
-      <c r="B41" t="str">
+      <c r="C41" t="str">
         <f>LOOKUP(A41,Analyses!$A$1:$B$401)</f>
         <v>Dm: Method invokes inefficient new String(String) constructor</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>110</v>
       </c>
-      <c r="B42" t="str">
+      <c r="C42" t="str">
         <f>LOOKUP(A42,Analyses!$A$1:$B$401)</f>
         <v>DMI: Vacuous call to collections</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>62</v>
       </c>
-      <c r="B43" t="str">
+      <c r="C43" t="str">
         <f>LOOKUP(A43,Analyses!$A$1:$B$401)</f>
         <v>OS: Method may fail to close stream on exception</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>328</v>
       </c>
-      <c r="B44" t="str">
+      <c r="C44" t="str">
         <f>LOOKUP(A44,Analyses!$A$1:$B$401)</f>
         <v>XSS: JSP reflected cross site scripting vulnerability</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>147</v>
       </c>
-      <c r="B45" t="str">
+      <c r="C45" t="str">
         <f>LOOKUP(A45,Analyses!$A$1:$B$401)</f>
         <v>IJU: TestCase has no tests</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>17</v>
       </c>
-      <c r="B46" t="str">
+      <c r="C46" t="str">
         <f>LOOKUP(A46,Analyses!$A$1:$B$401)</f>
         <v>ES: Comparison of String parameter using == or !=</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>248</v>
       </c>
-      <c r="B47" t="str">
+      <c r="C47" t="str">
         <f>LOOKUP(A47,Analyses!$A$1:$B$401)</f>
         <v>AT: Sequence of calls to concurrent abstraction may not be atomic</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>189</v>
       </c>
-      <c r="B48" t="str">
+      <c r="C48" t="str">
         <f>LOOKUP(A48,Analyses!$A$1:$B$401)</f>
         <v>RE: File.separator used for regular expression</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>383</v>
       </c>
-      <c r="B49" t="str">
+      <c r="C49" t="str">
         <f>LOOKUP(A49,Analyses!$A$1:$B$401)</f>
         <v>RV: Remainder of 32-bit signed random integer</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>15</v>
       </c>
-      <c r="B50" t="str">
+      <c r="C50" t="str">
         <f>LOOKUP(A50,Analyses!$A$1:$B$401)</f>
         <v>Dm: Method invokes System.exit(...)</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>119</v>
       </c>
-      <c r="B51" t="str">
+      <c r="C51" t="str">
         <f>LOOKUP(A51,Analyses!$A$1:$B$401)</f>
         <v>EC: Call to equals() comparing unrelated class and interface</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>108</v>
       </c>
-      <c r="B52" t="str">
+      <c r="C52" t="str">
         <f>LOOKUP(A52,Analyses!$A$1:$B$401)</f>
         <v>DMI: Invocation of hashCode on an array</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>225</v>
       </c>
-      <c r="B53" t="str">
+      <c r="C53" t="str">
         <f>LOOKUP(A53,Analyses!$A$1:$B$401)</f>
         <v>UwF: Field only ever set to null</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>335</v>
       </c>
-      <c r="B54" t="str">
+      <c r="C54" t="str">
         <f>LOOKUP(A54,Analyses!$A$1:$B$401)</f>
         <v>BC: instanceof will always return true</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>170</v>
       </c>
-      <c r="B55" t="str">
+      <c r="C55" t="str">
         <f>LOOKUP(A55,Analyses!$A$1:$B$401)</f>
         <v>NP: Method may return null, but is declared @NonNull</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>325</v>
       </c>
-      <c r="B56" t="str">
+      <c r="C56" t="str">
         <f>LOOKUP(A56,Analyses!$A$1:$B$401)</f>
         <v>PT: Relative path traversal in servlet</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>163</v>
       </c>
-      <c r="B57" t="str">
+      <c r="C57" t="str">
         <f>LOOKUP(A57,Analyses!$A$1:$B$401)</f>
         <v>NP: Null pointer dereference in method on exception path</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>391</v>
       </c>
-      <c r="B58" t="str">
+      <c r="C58" t="str">
         <f>LOOKUP(A58,Analyses!$A$1:$B$401)</f>
         <v>Se: private readResolve method not inherited by subclasses</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>20</v>
       </c>
-      <c r="B59" t="str">
+      <c r="C59" t="str">
         <f>LOOKUP(A59,Analyses!$A$1:$B$401)</f>
         <v>Eq: Equals checks for incompatible operand</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>218</v>
       </c>
-      <c r="B60" t="str">
+      <c r="C60" t="str">
         <f>LOOKUP(A60,Analyses!$A$1:$B$401)</f>
         <v>TQ: Value annotated as never carrying a type qualifier used where value carrying that qualifier is required</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>117</v>
       </c>
-      <c r="B61" t="str">
+      <c r="C61" t="str">
         <f>LOOKUP(A61,Analyses!$A$1:$B$401)</f>
         <v>EC: equals(...) used to compare incompatible arrays</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:3">
       <c r="A62">
         <v>77</v>
       </c>
-      <c r="B62" t="str">
+      <c r="C62" t="str">
         <f>LOOKUP(A62,Analyses!$A$1:$B$401)</f>
         <v>Se: serialVersionUID isn't final</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:3">
       <c r="A63">
         <v>340</v>
       </c>
-      <c r="B63" t="str">
+      <c r="C63" t="str">
         <f>LOOKUP(A63,Analyses!$A$1:$B$401)</f>
         <v>DLS: Dead store to local variable</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:3">
       <c r="A64">
         <v>46</v>
       </c>
-      <c r="B64" t="str">
+      <c r="C64" t="str">
         <f>LOOKUP(A64,Analyses!$A$1:$B$401)</f>
         <v>NP: equals() method does not check for null argument</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>278</v>
       </c>
-      <c r="B65" t="str">
+      <c r="C65" t="str">
         <f>LOOKUP(A65,Analyses!$A$1:$B$401)</f>
         <v>STCAL: Call to static DateFormat</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:3">
       <c r="A66">
         <v>380</v>
       </c>
-      <c r="B66" t="str">
+      <c r="C66" t="str">
         <f>LOOKUP(A66,Analyses!$A$1:$B$401)</f>
         <v>RV: Method checks to see if result of String.indexOf is positive</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:3">
       <c r="A67">
         <v>220</v>
       </c>
-      <c r="B67" t="str">
+      <c r="C67" t="str">
         <f>LOOKUP(A67,Analyses!$A$1:$B$401)</f>
         <v>UR: Uninitialized read of field in constructor</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:3">
       <c r="A68">
         <v>384</v>
       </c>
-      <c r="B68" t="str">
+      <c r="C68" t="str">
         <f>LOOKUP(A68,Analyses!$A$1:$B$401)</f>
         <v>RV: Method ignores return value, is this OK?</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:3">
       <c r="A69">
         <v>82</v>
       </c>
-      <c r="B69" t="str">
+      <c r="C69" t="str">
         <f>LOOKUP(A69,Analyses!$A$1:$B$401)</f>
         <v>Se: The readResolve method must be declared with a return type of Object.</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:3">
       <c r="A70">
         <v>323</v>
       </c>
-      <c r="B70" t="str">
+      <c r="C70" t="str">
         <f>LOOKUP(A70,Analyses!$A$1:$B$401)</f>
         <v>HRS: HTTP Response splitting vulnerability</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:3">
       <c r="A71">
         <v>297</v>
       </c>
-      <c r="B71" t="str">
+      <c r="C71" t="str">
         <f>LOOKUP(A71,Analyses!$A$1:$B$401)</f>
         <v>Bx: Method invokes inefficient floating-point Number constructor; use static valueOf instead</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:3">
       <c r="A72">
         <v>122</v>
       </c>
-      <c r="B72" t="str">
+      <c r="C72" t="str">
         <f>LOOKUP(A72,Analyses!$A$1:$B$401)</f>
         <v>EC: Using pointer equality to compare different types</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:3">
       <c r="A73">
         <v>114</v>
       </c>
-      <c r="B73" t="str">
+      <c r="C73" t="str">
         <f>LOOKUP(A73,Analyses!$A$1:$B$401)</f>
         <v>Dm: Useless/vacuous call to EasyMock method</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:3">
       <c r="A74">
         <v>399</v>
       </c>
-      <c r="B74" t="str">
+      <c r="C74" t="str">
         <f>LOOKUP(A74,Analyses!$A$1:$B$401)</f>
         <v>UwF: Field not initialized in constructor but dereferenced without null check</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:3">
       <c r="A75">
         <v>236</v>
       </c>
-      <c r="B75" t="str">
+      <c r="C75" t="str">
         <f>LOOKUP(A75,Analyses!$A$1:$B$401)</f>
         <v>EI2: May expose internal representation by incorporating reference to mutable object</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:3">
       <c r="A76">
         <v>396</v>
       </c>
-      <c r="B76" t="str">
+      <c r="C76" t="str">
         <f>LOOKUP(A76,Analyses!$A$1:$B$401)</f>
         <v>UCF: Useless control flow to next line</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:3">
       <c r="A77">
         <v>349</v>
       </c>
-      <c r="B77" t="str">
+      <c r="C77" t="str">
         <f>LOOKUP(A77,Analyses!$A$1:$B$401)</f>
         <v>Eq: Unusual equals method</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:3">
       <c r="A78">
         <v>3</v>
       </c>
-      <c r="B78" t="str">
+      <c r="C78" t="str">
         <f>LOOKUP(A78,Analyses!$A$1:$B$401)</f>
         <v>BC: Equals method should not assume anything about the type of its argument</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:3">
       <c r="A79">
         <v>337</v>
       </c>
-      <c r="B79" t="str">
+      <c r="C79" t="str">
         <f>LOOKUP(A79,Analyses!$A$1:$B$401)</f>
         <v>CI: Class is final but declares protected field</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:3">
       <c r="A80">
         <v>280</v>
       </c>
-      <c r="B80" t="str">
+      <c r="C80" t="str">
         <f>LOOKUP(A80,Analyses!$A$1:$B$401)</f>
         <v>STCAL: Static DateFormat</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:3">
       <c r="A81">
         <v>5</v>
       </c>
-      <c r="B81" t="str">
+      <c r="C81" t="str">
         <f>LOOKUP(A81,Analyses!$A$1:$B$401)</f>
         <v>CN: Class implements Cloneable but does not define or use clone method</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:3">
       <c r="A82">
         <v>260</v>
       </c>
-      <c r="B82" t="str">
+      <c r="C82" t="str">
         <f>LOOKUP(A82,Analyses!$A$1:$B$401)</f>
         <v>JLM: Synchronization performed on util.concurrent instance</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:3">
       <c r="A83">
         <v>76</v>
       </c>
-      <c r="B83" t="str">
+      <c r="C83" t="str">
         <f>LOOKUP(A83,Analyses!$A$1:$B$401)</f>
         <v>Se: Serializable inner class</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:3">
       <c r="A84">
         <v>203</v>
       </c>
-      <c r="B84" t="str">
+      <c r="C84" t="str">
         <f>LOOKUP(A84,Analyses!$A$1:$B$401)</f>
         <v>SA: Nonsensical self computation involving a variable (e.g., x &amp; x)</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:3">
       <c r="A85">
         <v>60</v>
       </c>
-      <c r="B85" t="str">
+      <c r="C85" t="str">
         <f>LOOKUP(A85,Analyses!$A$1:$B$401)</f>
         <v>ODR: Method may fail to close database resource on exception</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:3">
       <c r="A86">
         <v>192</v>
       </c>
-      <c r="B86" t="str">
+      <c r="C86" t="str">
         <f>LOOKUP(A86,Analyses!$A$1:$B$401)</f>
         <v>RV: Bad attempt to compute absolute value of signed 32-bit hashcode</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:3">
       <c r="A87">
         <v>90</v>
       </c>
-      <c r="B87" t="str">
+      <c r="C87" t="str">
         <f>LOOKUP(A87,Analyses!$A$1:$B$401)</f>
         <v>BIT: Bitwise add of signed byte value</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:3">
       <c r="A88">
         <v>58</v>
       </c>
-      <c r="B88" t="str">
+      <c r="C88" t="str">
         <f>LOOKUP(A88,Analyses!$A$1:$B$401)</f>
         <v>Nm: Method doesn't override method in superclass due to wrong package for parameter</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:3">
       <c r="A89">
         <v>301</v>
       </c>
-      <c r="B89" t="str">
+      <c r="C89" t="str">
         <f>LOOKUP(A89,Analyses!$A$1:$B$401)</f>
         <v>Dm: Method invokes inefficient Boolean constructor; use Boolean.valueOf(...) instead</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:3">
       <c r="A90">
         <v>54</v>
       </c>
-      <c r="B90" t="str">
+      <c r="C90" t="str">
         <f>LOOKUP(A90,Analyses!$A$1:$B$401)</f>
         <v>Nm: Method names should start with a lower case letter</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:3">
       <c r="A91">
         <v>190</v>
       </c>
-      <c r="B91" t="str">
+      <c r="C91" t="str">
         <f>LOOKUP(A91,Analyses!$A$1:$B$401)</f>
         <v>RE: "." used for regular expression</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:3">
       <c r="A92">
         <v>299</v>
       </c>
-      <c r="B92" t="str">
+      <c r="C92" t="str">
         <f>LOOKUP(A92,Analyses!$A$1:$B$401)</f>
         <v>Dm: The equals and hashCode methods of URL are blocking</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:3">
       <c r="A93">
         <v>315</v>
       </c>
-      <c r="B93" t="str">
+      <c r="C93" t="str">
         <f>LOOKUP(A93,Analyses!$A$1:$B$401)</f>
         <v>UM: Method calls static Math class method on a constant value</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:3">
       <c r="A94">
         <v>12</v>
       </c>
-      <c r="B94" t="str">
+      <c r="C94" t="str">
         <f>LOOKUP(A94,Analyses!$A$1:$B$401)</f>
         <v>DMI: Adding elements of an entry set may fail due to reuse of Entry objects</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:3">
       <c r="A95">
         <v>37</v>
       </c>
-      <c r="B95" t="str">
+      <c r="C95" t="str">
         <f>LOOKUP(A95,Analyses!$A$1:$B$401)</f>
         <v>HE: Class inherits equals() and uses Object.hashCode()</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:3">
       <c r="A96">
         <v>16</v>
       </c>
-      <c r="B96" t="str">
+      <c r="C96" t="str">
         <f>LOOKUP(A96,Analyses!$A$1:$B$401)</f>
         <v>Dm: Method invokes dangerous method runFinalizersOnExit</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:3">
       <c r="A97">
         <v>360</v>
       </c>
-      <c r="B97" t="str">
+      <c r="C97" t="str">
         <f>LOOKUP(A97,Analyses!$A$1:$B$401)</f>
         <v>INT: Vacuous comparison of integer value</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:3">
       <c r="A98">
         <v>49</v>
       </c>
-      <c r="B98" t="str">
+      <c r="C98" t="str">
         <f>LOOKUP(A98,Analyses!$A$1:$B$401)</f>
         <v>Nm: Class is not derived from an Exception, even though it is named as such</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:3">
       <c r="A99">
         <v>56</v>
       </c>
-      <c r="B99" t="str">
+      <c r="C99" t="str">
         <f>LOOKUP(A99,Analyses!$A$1:$B$401)</f>
         <v>Nm: Class names shouldn't shadow simple name of superclass</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:3">
       <c r="A100">
         <v>284</v>
       </c>
-      <c r="B100" t="str">
+      <c r="C100" t="str">
         <f>LOOKUP(A100,Analyses!$A$1:$B$401)</f>
         <v>UL: Method does not release lock on all paths</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:3">
       <c r="A101">
         <v>111</v>
       </c>
-      <c r="B101" t="str">
+      <c r="C101" t="str">
         <f>LOOKUP(A101,Analyses!$A$1:$B$401)</f>
         <v>Dm: Can't use reflection to check for presence of annotation without runtime retention</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:3">
       <c r="A102">
         <v>195</v>
       </c>
-      <c r="B102" t="str">
+      <c r="C102" t="str">
         <f>LOOKUP(A102,Analyses!$A$1:$B$401)</f>
         <v>RV: Exception created and dropped rather than thrown</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:3">
       <c r="A103">
         <v>346</v>
       </c>
-      <c r="B103" t="str">
+      <c r="C103" t="str">
         <f>LOOKUP(A103,Analyses!$A$1:$B$401)</f>
         <v>DMI: Invocation of substring(0), which returns the original value</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:3">
       <c r="A104">
         <v>129</v>
       </c>
-      <c r="B104" t="str">
+      <c r="C104" t="str">
         <f>LOOKUP(A104,Analyses!$A$1:$B$401)</f>
         <v>Eq: equals method overrides equals in superclass and may not be symmetric</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:3">
       <c r="A105">
         <v>137</v>
       </c>
-      <c r="B105" t="str">
+      <c r="C105" t="str">
         <f>LOOKUP(A105,Analyses!$A$1:$B$401)</f>
         <v>FS: Format string references missing argument</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:3">
       <c r="A106">
         <v>118</v>
       </c>
-      <c r="B106" t="str">
+      <c r="C106" t="str">
         <f>LOOKUP(A106,Analyses!$A$1:$B$401)</f>
         <v>EC: Call to equals(null)</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:3">
       <c r="A107">
         <v>157</v>
       </c>
-      <c r="B107" t="str">
+      <c r="C107" t="str">
         <f>LOOKUP(A107,Analyses!$A$1:$B$401)</f>
         <v>INT: Bad comparison of signed byte</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:3">
       <c r="A108">
         <v>311</v>
       </c>
-      <c r="B108" t="str">
+      <c r="C108" t="str">
         <f>LOOKUP(A108,Analyses!$A$1:$B$401)</f>
         <v>SIC: Should be a static inner class</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:3">
       <c r="A109">
         <v>35</v>
       </c>
-      <c r="B109" t="str">
+      <c r="C109" t="str">
         <f>LOOKUP(A109,Analyses!$A$1:$B$401)</f>
         <v>HE: Class defines hashCode() but not equals()</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:3">
       <c r="A110">
         <v>78</v>
       </c>
-      <c r="B110" t="str">
+      <c r="C110" t="str">
         <f>LOOKUP(A110,Analyses!$A$1:$B$401)</f>
         <v>Se: serialVersionUID isn't long</v>
       </c>
@@ -7962,7 +8007,7 @@
     <sortCondition ref="A127"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added some further information
</commit_message>
<xml_diff>
--- a/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
+++ b/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="455">
   <si>
     <t>AM: Creates an empty jar file entry</t>
   </si>
@@ -1404,12 +1404,15 @@
   <si>
     <t>Implemented</t>
   </si>
+  <si>
+    <t>FI_USELESS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1511,6 +1514,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Zapf Dingbats"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1566,7 +1576,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1580,6 +1590,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6376,8 +6389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6456,24 +6469,27 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12">
+    <row r="12" spans="1:9" s="10" customFormat="1">
+      <c r="A12" s="10">
         <v>312</v>
       </c>
-      <c r="C12" t="str">
+      <c r="B12" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="C12" s="10" t="str">
         <f>LOOKUP(A12,Analyses!$A$1:$B$401)</f>
         <v>SIC: Could be refactored into a named static inner class</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="10" t="s">
         <v>435</v>
       </c>
     </row>
@@ -6495,87 +6511,96 @@
         <v>439</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14">
+    <row r="14" spans="1:9" s="10" customFormat="1">
+      <c r="A14" s="10">
         <v>309</v>
       </c>
-      <c r="C14" t="str">
+      <c r="B14" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="C14" s="10" t="str">
         <f>LOOKUP(A14,Analyses!$A$1:$B$401)</f>
         <v>ITA: Method uses toArray() with zero-length array argument</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="10" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15">
+    <row r="15" spans="1:9" s="10" customFormat="1">
+      <c r="A15" s="10">
         <v>109</v>
       </c>
-      <c r="C15" t="str">
+      <c r="B15" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="C15" s="10" t="str">
         <f>LOOKUP(A15,Analyses!$A$1:$B$401)</f>
         <v>DMI: Double.longBitsToDouble invoked on an int</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="10" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16">
-      <c r="A16">
+    <row r="16" spans="1:9" s="10" customFormat="1" ht="16">
+      <c r="A16" s="10">
         <v>245</v>
       </c>
-      <c r="C16" t="str">
+      <c r="B16" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="C16" s="10" t="str">
         <f>LOOKUP(A16,Analyses!$A$1:$B$401)</f>
         <v>MS: Field should be package protected</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="10" t="s">
         <v>445</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17">
+    <row r="17" spans="1:9" s="13" customFormat="1">
+      <c r="A17" s="13">
         <v>251</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="13" t="str">
         <f>LOOKUP(A17,Analyses!$A$1:$B$401)</f>
         <v>DL: Synchronization on boxed primitive</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="13" t="s">
         <v>447</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="14" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18">
+    <row r="18" spans="1:9" s="1" customFormat="1">
+      <c r="A18" s="1">
         <v>221</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18" s="1" t="str">
         <f>LOOKUP(A18,Analyses!$A$1:$B$401)</f>
         <v>UR: Uninitialized read of field method called from constructor of superclass</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="15" t="s">
         <v>420</v>
       </c>
     </row>
@@ -6633,15 +6658,18 @@
         <v>418</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22">
+    <row r="22" spans="1:9" s="1" customFormat="1">
+      <c r="A22" s="1">
         <v>30</v>
       </c>
-      <c r="C22" t="str">
+      <c r="C22" s="1" t="str">
         <f>LOOKUP(A22,Analyses!$A$1:$B$401)</f>
         <v>FI: Finalizer does nothing but call superclass finalizer</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="D22" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>420</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated implemented analyses list
</commit_message>
<xml_diff>
--- a/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
+++ b/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38300" yWindow="-380" windowWidth="38320" windowHeight="23560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-38295" yWindow="-375" windowWidth="20730" windowHeight="23565" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analyses" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="SQL_BAD_PREPARED_STATEMENT_ACCESS" localSheetId="1">'ausgewählte Analysen'!$D$13</definedName>
     <definedName name="UR_UNINIT_READ_CALLED_FROM_SUPER_CONSTRUCTOR" localSheetId="1">'ausgewählte Analysen'!$D$18</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="455">
   <si>
     <t>AM: Creates an empty jar file entry</t>
   </si>
@@ -1412,7 +1412,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1521,6 +1521,14 @@
       <name val="Zapf Dingbats"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1576,7 +1584,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1593,19 +1601,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1617,7 +1626,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1957,9 +1966,9 @@
       <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="90.1640625" customWidth="1"/>
+    <col min="2" max="2" width="90.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6387,22 +6396,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I226"/>
+  <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="31.625" customWidth="1"/>
+    <col min="3" max="3" width="71.375" customWidth="1"/>
+    <col min="4" max="4" width="29.625" customWidth="1"/>
+    <col min="7" max="7" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>404</v>
       </c>
@@ -6442,7 +6451,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>411</v>
       </c>
@@ -6556,7 +6565,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="10" customFormat="1" ht="16">
+    <row r="16" spans="1:9" s="10" customFormat="1">
       <c r="A16" s="10">
         <v>245</v>
       </c>
@@ -6574,7 +6583,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="13" customFormat="1">
+    <row r="17" spans="1:10" s="13" customFormat="1">
       <c r="A17" s="13">
         <v>251</v>
       </c>
@@ -6589,22 +6598,30 @@
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="1" customFormat="1">
-      <c r="A18" s="1">
+    <row r="18" spans="1:10" s="1" customFormat="1">
+      <c r="A18" s="10">
         <v>221</v>
       </c>
-      <c r="C18" s="1" t="str">
+      <c r="B18" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="C18" s="10" t="str">
         <f>LOOKUP(A18,Analyses!$A$1:$B$401)</f>
         <v>UR: Uninitialized read of field method called from constructor of superclass</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="10" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>201</v>
       </c>
@@ -6622,7 +6639,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="10" customFormat="1">
+    <row r="20" spans="1:10" s="10" customFormat="1">
       <c r="A20" s="10">
         <v>73</v>
       </c>
@@ -6640,7 +6657,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="12" customFormat="1">
+    <row r="21" spans="1:10" s="12" customFormat="1">
       <c r="A21" s="12">
         <v>177</v>
       </c>
@@ -6658,7 +6675,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1">
+    <row r="22" spans="1:10" s="1" customFormat="1">
       <c r="A22" s="1">
         <v>30</v>
       </c>
@@ -6673,19 +6690,19 @@
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16">
-      <c r="A23">
+    <row r="23" spans="1:10" s="1" customFormat="1">
+      <c r="A23" s="1">
         <v>71</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C23" s="1" t="str">
         <f>LOOKUP(A23,Analyses!$A$1:$B$401)</f>
         <v>SW: Certain swing methods needs to be invoked in Swing thread</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="16" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>267</v>
       </c>
@@ -6697,7 +6714,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>246</v>
       </c>
@@ -6709,7 +6726,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="16">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>234</v>
       </c>
@@ -6721,7 +6738,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="16">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>387</v>
       </c>
@@ -6733,7 +6750,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>199</v>
       </c>
@@ -6745,7 +6762,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>294</v>
       </c>
@@ -6757,7 +6774,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>223</v>
       </c>
@@ -6772,7 +6789,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>196</v>
       </c>
@@ -6784,7 +6801,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="16">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>69</v>
       </c>
@@ -6808,7 +6825,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="16">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>10</v>
       </c>
@@ -6856,7 +6873,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="16">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>41</v>
       </c>
@@ -8035,7 +8052,7 @@
     <sortCondition ref="A127"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated list of implemented checkers
</commit_message>
<xml_diff>
--- a/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
+++ b/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="455">
   <si>
     <t>AM: Creates an empty jar file entry</t>
   </si>
@@ -1412,7 +1412,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1521,14 +1521,6 @@
       <name val="Zapf Dingbats"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1584,7 +1576,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1601,7 +1593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6399,7 +6390,7 @@
   <dimension ref="A1:J226"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -6690,15 +6681,18 @@
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="1" customFormat="1">
-      <c r="A23" s="1">
+    <row r="23" spans="1:10" s="10" customFormat="1">
+      <c r="A23" s="10">
         <v>71</v>
       </c>
-      <c r="C23" s="1" t="str">
+      <c r="B23" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="C23" s="10" t="str">
         <f>LOOKUP(A23,Analyses!$A$1:$B$401)</f>
         <v>SW: Certain swing methods needs to be invoked in Swing thread</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="10" t="s">
         <v>422</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added checker for fields that should be final
</commit_message>
<xml_diff>
--- a/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
+++ b/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
@@ -15,6 +15,8 @@
     <definedName name="DMI_LONG_BITS_TO_DOUBLE_INVOKED_ON_INT" localSheetId="1">'ausgewählte Analysen'!$D$15</definedName>
     <definedName name="ITA_INEFFICIENT_TO_ARRAY" localSheetId="1">'ausgewählte Analysen'!$D$14</definedName>
     <definedName name="MS_PKGPROTECT" localSheetId="1">'ausgewählte Analysen'!$D$16</definedName>
+    <definedName name="MS_SHOULD_BE_FINAL" localSheetId="1">'ausgewählte Analysen'!$D$25</definedName>
+    <definedName name="MWN_MISMATCHED_NOTIFY" localSheetId="1">'ausgewählte Analysen'!$D$24</definedName>
     <definedName name="RC_REF_COMPARISON" localSheetId="1">'ausgewählte Analysen'!$D$11</definedName>
     <definedName name="SA_LOCAL_SELF_ASSIGNMENT_INSTEAD_OF_FIELD" localSheetId="1">'ausgewählte Analysen'!$D$19</definedName>
     <definedName name="SIC_INNER_SHOULD_BE_STATIC_ANON" localSheetId="1">'ausgewählte Analysen'!$D$12</definedName>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="459">
   <si>
     <t>AM: Creates an empty jar file entry</t>
   </si>
@@ -1300,9 +1302,6 @@
   </si>
   <si>
     <t>Study of the implementation is necessary!</t>
-  </si>
-  <si>
-    <t>Scope is not 100% clear</t>
   </si>
   <si>
     <t>Needs IMCF (to determine which instructions are executed within a synchronized block) - could use GCF to reduce # of false warnings</t>
@@ -1407,12 +1406,27 @@
   <si>
     <t>FI_USELESS</t>
   </si>
+  <si>
+    <t>SW_SWING_METHODS_INVOKED_IN_SWING_THREAD</t>
+  </si>
+  <si>
+    <t>MWN_MISMATCHED_NOTIFY</t>
+  </si>
+  <si>
+    <t>MS_SHOULD_BE_FINAL</t>
+  </si>
+  <si>
+    <t>Calls to pack/show/setVisible in main method or (curiously) in classes called *benchmark*</t>
+  </si>
+  <si>
+    <t>Reports a bug if: field is public/protected static !final !Array &amp;&amp; !Hashtable</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1521,6 +1535,14 @@
       <name val="Zapf Dingbats"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1576,7 +1598,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1593,6 +1615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6389,8 +6412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -6448,10 +6471,10 @@
       </c>
       <c r="B10" s="1"/>
       <c r="H10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -6463,7 +6486,7 @@
         <v>RC: Suspicious reference comparison</v>
       </c>
       <c r="D11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>413</v>
@@ -6474,23 +6497,23 @@
         <v>312</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C12" s="10" t="str">
         <f>LOOKUP(A12,Analyses!$A$1:$B$401)</f>
         <v>SIC: Could be refactored into a named static inner class</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>416</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -6502,13 +6525,13 @@
         <v>SQL: Method attempts to access a prepared statement parameter with index 0</v>
       </c>
       <c r="D13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E13" t="s">
         <v>417</v>
       </c>
       <c r="I13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="10" customFormat="1">
@@ -6516,23 +6539,23 @@
         <v>309</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C14" s="10" t="str">
         <f>LOOKUP(A14,Analyses!$A$1:$B$401)</f>
         <v>ITA: Method uses toArray() with zero-length array argument</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>418</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="10" customFormat="1">
@@ -6540,20 +6563,20 @@
         <v>109</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C15" s="10" t="str">
         <f>LOOKUP(A15,Analyses!$A$1:$B$401)</f>
         <v>DMI: Double.longBitsToDouble invoked on an int</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>419</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="10" customFormat="1">
@@ -6561,17 +6584,17 @@
         <v>245</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C16" s="10" t="str">
         <f>LOOKUP(A16,Analyses!$A$1:$B$401)</f>
         <v>MS: Field should be package protected</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>445</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="13" customFormat="1">
@@ -6583,7 +6606,7 @@
         <v>DL: Synchronization on boxed primitive</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>413</v>
@@ -6594,14 +6617,14 @@
         <v>221</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C18" s="10" t="str">
         <f>LOOKUP(A18,Analyses!$A$1:$B$401)</f>
         <v>UR: Uninitialized read of field method called from constructor of superclass</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>420</v>
@@ -6621,13 +6644,13 @@
         <v>SA: Self assignment of local rather than assignment to field</v>
       </c>
       <c r="D19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E19" t="s">
         <v>421</v>
       </c>
       <c r="I19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="10" customFormat="1">
@@ -6635,14 +6658,14 @@
         <v>73</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C20" s="10" t="str">
         <f>LOOKUP(A20,Analyses!$A$1:$B$401)</f>
         <v>Se: Non-serializable class has a serializable inner class</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>420</v>
@@ -6660,7 +6683,7 @@
         <v>NP: Store of null value into field annotated NonNull</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>418</v>
@@ -6675,7 +6698,7 @@
         <v>FI: Finalizer does nothing but call superclass finalizer</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>420</v>
@@ -6686,14 +6709,17 @@
         <v>71</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C23" s="10" t="str">
         <f>LOOKUP(A23,Analyses!$A$1:$B$401)</f>
         <v>SW: Certain swing methods needs to be invoked in Swing thread</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>422</v>
+      <c r="D23" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -6704,20 +6730,29 @@
         <f>LOOKUP(A24,Analyses!$A$1:$B$401)</f>
         <v>MWN: Mismatched notify()</v>
       </c>
+      <c r="D24" t="s">
+        <v>455</v>
+      </c>
       <c r="E24" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="10" customFormat="1">
+      <c r="A25" s="10">
         <v>246</v>
       </c>
-      <c r="C25" t="str">
+      <c r="B25" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="C25" s="10" t="str">
         <f>LOOKUP(A25,Analyses!$A$1:$B$401)</f>
         <v>MS: Field isn't final but should be</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>423</v>
+      <c r="D25" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -6741,7 +6776,7 @@
         <v>SA: Self assignment of local variable</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -6765,7 +6800,7 @@
         <v>Bx: Primitive value is boxed then unboxed to perform primitive coercion</v>
       </c>
       <c r="E29" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -6777,10 +6812,10 @@
         <v>USELESS_STRING: Invocation of toString on an array</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H30" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6792,7 +6827,7 @@
         <v>RV: Method ignores return value</v>
       </c>
       <c r="E31" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6804,7 +6839,7 @@
         <v>RV: Method ignores exceptional return value</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -6888,7 +6923,7 @@
         <v>TQ: Value required to have type qualifier, but marked as unknown</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="40" spans="1:5">

</xml_diff>

<commit_message>
preliminary implementation of the checker
</commit_message>
<xml_diff>
--- a/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
+++ b/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38295" yWindow="-375" windowWidth="20730" windowHeight="23565" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-36200" yWindow="-360" windowWidth="28220" windowHeight="23560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analyses" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="SQL_BAD_PREPARED_STATEMENT_ACCESS" localSheetId="1">'ausgewählte Analysen'!$D$13</definedName>
     <definedName name="UR_UNINIT_READ_CALLED_FROM_SUPER_CONSTRUCTOR" localSheetId="1">'ausgewählte Analysen'!$D$18</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="459">
   <si>
     <t>AM: Creates an empty jar file entry</t>
   </si>
@@ -1426,7 +1426,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1531,13 +1531,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Zapf Dingbats"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="6" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1598,7 +1591,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1615,20 +1608,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1640,7 +1632,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1980,9 +1972,9 @@
       <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="90.125" customWidth="1"/>
+    <col min="2" max="2" width="90.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6412,20 +6404,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="31.625" customWidth="1"/>
-    <col min="3" max="3" width="71.375" customWidth="1"/>
-    <col min="4" max="4" width="29.625" customWidth="1"/>
-    <col min="7" max="7" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="71.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="16">
       <c r="A1" s="1" t="s">
         <v>404</v>
       </c>
@@ -6465,7 +6457,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="16">
       <c r="A10" s="1" t="s">
         <v>411</v>
       </c>
@@ -6579,7 +6571,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="10" customFormat="1">
+    <row r="16" spans="1:9" s="10" customFormat="1" ht="16">
       <c r="A16" s="10">
         <v>245</v>
       </c>
@@ -6612,7 +6604,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1">
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="16">
       <c r="A18" s="10">
         <v>221</v>
       </c>
@@ -6689,18 +6681,21 @@
         <v>418</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1">
-      <c r="A22" s="1">
+    <row r="22" spans="1:10" s="10" customFormat="1">
+      <c r="A22" s="10">
         <v>30</v>
       </c>
-      <c r="C22" s="1" t="str">
+      <c r="B22" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="C22" s="10" t="str">
         <f>LOOKUP(A22,Analyses!$A$1:$B$401)</f>
         <v>FI: Finalizer does nothing but call superclass finalizer</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="11" t="s">
         <v>420</v>
       </c>
     </row>
@@ -6737,7 +6732,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="10" customFormat="1">
+    <row r="25" spans="1:10" s="10" customFormat="1" ht="16">
       <c r="A25" s="10">
         <v>246</v>
       </c>
@@ -6751,11 +6746,11 @@
       <c r="D25" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="15" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" ht="16">
       <c r="A26">
         <v>234</v>
       </c>
@@ -6767,7 +6762,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" ht="16">
       <c r="A27">
         <v>387</v>
       </c>
@@ -6830,7 +6825,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" ht="16">
       <c r="A32">
         <v>69</v>
       </c>
@@ -6854,7 +6849,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" ht="16">
       <c r="A34">
         <v>10</v>
       </c>
@@ -6902,7 +6897,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" ht="16">
       <c r="A38">
         <v>41</v>
       </c>
@@ -8081,7 +8076,7 @@
     <sortCondition ref="A127"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated list of implemented analyses
</commit_message>
<xml_diff>
--- a/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
+++ b/demo/src/main/scala/de/tud/cs/st/bat/resolved/analyses/Chosing the Findbugs Analyses.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36200" yWindow="-360" windowWidth="28220" windowHeight="23560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-36195" yWindow="-360" windowWidth="20730" windowHeight="23565" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analyses" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="SQL_BAD_PREPARED_STATEMENT_ACCESS" localSheetId="1">'ausgewählte Analysen'!$D$13</definedName>
     <definedName name="UR_UNINIT_READ_CALLED_FROM_SUPER_CONSTRUCTOR" localSheetId="1">'ausgewählte Analysen'!$D$18</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="460">
   <si>
     <t>AM: Creates an empty jar file entry</t>
   </si>
@@ -1421,12 +1421,15 @@
   <si>
     <t>Reports a bug if: field is public/protected static !final !Array &amp;&amp; !Hashtable</t>
   </si>
+  <si>
+    <t>BX_BOXING_IMMEDIATELY_UNBOXED_TO_PERFORM_COERCION</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1610,17 +1613,17 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1632,7 +1635,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1972,9 +1975,9 @@
       <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="90.1640625" customWidth="1"/>
+    <col min="2" max="2" width="90.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6404,20 +6407,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="31.625" customWidth="1"/>
+    <col min="3" max="3" width="71.375" customWidth="1"/>
+    <col min="4" max="4" width="29.625" customWidth="1"/>
+    <col min="7" max="7" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>404</v>
       </c>
@@ -6457,7 +6460,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>411</v>
       </c>
@@ -6571,7 +6574,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="10" customFormat="1" ht="16">
+    <row r="16" spans="1:9" s="10" customFormat="1">
       <c r="A16" s="10">
         <v>245</v>
       </c>
@@ -6604,7 +6607,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="16">
+    <row r="18" spans="1:10" s="1" customFormat="1">
       <c r="A18" s="10">
         <v>221</v>
       </c>
@@ -6732,7 +6735,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="10" customFormat="1" ht="16">
+    <row r="25" spans="1:10" s="10" customFormat="1">
       <c r="A25" s="10">
         <v>246</v>
       </c>
@@ -6750,7 +6753,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>234</v>
       </c>
@@ -6762,7 +6765,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="16">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>387</v>
       </c>
@@ -6786,15 +6789,21 @@
         <v>418</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
-      <c r="A29">
+    <row r="29" spans="1:10" s="10" customFormat="1">
+      <c r="A29" s="10">
         <v>294</v>
       </c>
-      <c r="C29" t="str">
+      <c r="B29" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="C29" s="10" t="str">
         <f>LOOKUP(A29,Analyses!$A$1:$B$401)</f>
         <v>Bx: Primitive value is boxed then unboxed to perform primitive coercion</v>
       </c>
-      <c r="E29" t="s">
+      <c r="D29" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="E29" s="10" t="s">
         <v>425</v>
       </c>
     </row>
@@ -6825,7 +6834,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="16">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>69</v>
       </c>
@@ -6849,7 +6858,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="16">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>10</v>
       </c>
@@ -6897,7 +6906,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="16">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>41</v>
       </c>

</xml_diff>